<commit_message>
feat: Fixed failing test cases by changing the file structure
</commit_message>
<xml_diff>
--- a/src/integrationTest/resources/Staff Data Upload With Jsr.xlsx
+++ b/src/integrationTest/resources/Staff Data Upload With Jsr.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m_224557/Documents/GitHub/duplicate/rd-caseworker-ref-api/src/integrationTest/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDC29247-AA22-0D40-87BE-8A79EF8DFD9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F5C3818-588F-1440-9D32-C122B1E1E883}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19520" activeTab="2" xr2:uid="{C3779BBE-D7A5-4756-9223-DEADF9C5B8AB}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1952" uniqueCount="1226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1924" uniqueCount="1217">
   <si>
     <t>Region</t>
   </si>
@@ -3658,9 +3658,6 @@
     <t>lastsecond</t>
   </si>
   <si>
-    <t>test@domain.com</t>
-  </si>
-  <si>
     <t>testthird</t>
   </si>
   <si>
@@ -3698,30 +3695,6 @@
   </si>
   <si>
     <t>testeight@justice.gov.uk</t>
-  </si>
-  <si>
-    <t>testnine</t>
-  </si>
-  <si>
-    <t>lastnine</t>
-  </si>
-  <si>
-    <t>testnine@justice.gov.uk</t>
-  </si>
-  <si>
-    <t>testten</t>
-  </si>
-  <si>
-    <t>testten@justice.gov.uk</t>
-  </si>
-  <si>
-    <t>testeleven</t>
-  </si>
-  <si>
-    <t>lasteleven</t>
-  </si>
-  <si>
-    <t>testeleven@justice.gov.uk</t>
   </si>
 </sst>
 </file>
@@ -7720,7 +7693,7 @@
   <dimension ref="A1:AD50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7874,11 +7847,11 @@
         <v>219164</v>
       </c>
       <c r="H2" s="41" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="I2" s="1">
         <f>_xlfn.IFNA(VLOOKUP(H2,'Base Locations'!A1:F341,2),"")</f>
-        <v>817181</v>
+        <v>574546</v>
       </c>
       <c r="J2" s="41" t="s">
         <v>52</v>
@@ -7944,7 +7917,7 @@
         <v>1203</v>
       </c>
       <c r="C3" s="42" t="s">
-        <v>1204</v>
+        <v>1201</v>
       </c>
       <c r="D3" s="41" t="s">
         <v>5</v>
@@ -8019,13 +7992,13 @@
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A4" s="41" t="s">
+        <v>1204</v>
+      </c>
+      <c r="B4" s="41" t="s">
         <v>1205</v>
       </c>
-      <c r="B4" s="41" t="s">
+      <c r="C4" s="42" t="s">
         <v>1206</v>
-      </c>
-      <c r="C4" s="42" t="s">
-        <v>1207</v>
       </c>
       <c r="D4" s="41" t="s">
         <v>10</v>
@@ -8102,13 +8075,13 @@
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A5" s="41" t="s">
+        <v>1207</v>
+      </c>
+      <c r="B5" s="41" t="s">
         <v>1208</v>
       </c>
-      <c r="B5" s="41" t="s">
+      <c r="C5" s="42" t="s">
         <v>1209</v>
-      </c>
-      <c r="C5" s="42" t="s">
-        <v>1210</v>
       </c>
       <c r="D5" s="41" t="s">
         <v>6</v>
@@ -8183,13 +8156,13 @@
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A6" s="41" t="s">
+        <v>1207</v>
+      </c>
+      <c r="B6" s="41" t="s">
         <v>1208</v>
       </c>
-      <c r="B6" s="41" t="s">
+      <c r="C6" s="42" t="s">
         <v>1209</v>
-      </c>
-      <c r="C6" s="42" t="s">
-        <v>1210</v>
       </c>
       <c r="D6" s="41" t="s">
         <v>5</v>
@@ -8263,10 +8236,10 @@
     <row r="7" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A7" s="41"/>
       <c r="B7" s="41" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="C7" s="42" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="D7" s="41" t="s">
         <v>5</v>
@@ -8343,11 +8316,11 @@
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A8" s="41" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
       <c r="B8" s="41"/>
       <c r="C8" s="42" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="D8" s="41" t="s">
         <v>11</v>
@@ -8422,10 +8395,10 @@
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A9" s="41" t="s">
+        <v>1212</v>
+      </c>
+      <c r="B9" s="41" t="s">
         <v>1213</v>
-      </c>
-      <c r="B9" s="41" t="s">
-        <v>1214</v>
       </c>
       <c r="C9" s="42"/>
       <c r="D9" s="41" t="s">
@@ -8503,13 +8476,13 @@
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A10" s="41" t="s">
+        <v>1214</v>
+      </c>
+      <c r="B10" s="41" t="s">
         <v>1215</v>
       </c>
-      <c r="B10" s="41" t="s">
+      <c r="C10" s="42" t="s">
         <v>1216</v>
-      </c>
-      <c r="C10" s="42" t="s">
-        <v>1217</v>
       </c>
       <c r="D10" s="41"/>
       <c r="E10" s="1" t="str">
@@ -8583,51 +8556,31 @@
       <c r="AD10" s="41"/>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A11" s="41" t="s">
-        <v>1218</v>
-      </c>
-      <c r="B11" s="41" t="s">
-        <v>1219</v>
-      </c>
-      <c r="C11" s="42" t="s">
-        <v>1220</v>
-      </c>
-      <c r="D11" s="41" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="1">
+      <c r="A11" s="41"/>
+      <c r="B11" s="41"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="1" t="str">
         <f>_xlfn.IFNA(VLOOKUP(D11,Region!$A$2:$B$11,2),"")</f>
-        <v>5</v>
-      </c>
-      <c r="F11" s="41" t="s">
-        <v>70</v>
-      </c>
-      <c r="G11" s="1">
+        <v/>
+      </c>
+      <c r="F11" s="41"/>
+      <c r="G11" s="1" t="str">
         <f>_xlfn.IFNA(VLOOKUP(F11,'Base Locations'!$A$1:$F$341,2),"")</f>
-        <v>827534</v>
-      </c>
-      <c r="H11" s="41" t="s">
-        <v>74</v>
-      </c>
+        <v/>
+      </c>
+      <c r="H11" s="41"/>
       <c r="I11" s="1" t="str">
         <f>_xlfn.IFNA(VLOOKUP(H11,'Base Locations'!A10:F350,2),"")</f>
         <v/>
       </c>
-      <c r="J11" s="41" t="s">
-        <v>52</v>
-      </c>
-      <c r="K11" s="41" t="s">
-        <v>409</v>
-      </c>
-      <c r="L11" s="41" t="s">
-        <v>409</v>
-      </c>
-      <c r="M11" s="41" t="s">
-        <v>13</v>
-      </c>
+      <c r="J11" s="41"/>
+      <c r="K11" s="41"/>
+      <c r="L11" s="41"/>
+      <c r="M11" s="41"/>
       <c r="N11" s="1" t="str">
         <f>_xlfn.IFNA(VLOOKUP(M11,Services!$A$1:$B$45,2),"")</f>
-        <v>BAB1</v>
+        <v/>
       </c>
       <c r="O11" s="41"/>
       <c r="P11" s="1" t="str">
@@ -8668,49 +8621,31 @@
       <c r="AD11" s="41"/>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A12" s="41" t="s">
-        <v>1221</v>
-      </c>
-      <c r="B12" s="41" t="s">
-        <v>1221</v>
-      </c>
-      <c r="C12" s="42" t="s">
-        <v>1222</v>
-      </c>
-      <c r="D12" s="41" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" s="1">
+      <c r="A12" s="41"/>
+      <c r="B12" s="41"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="1" t="str">
         <f>_xlfn.IFNA(VLOOKUP(D12,Region!$A$2:$B$11,2),"")</f>
-        <v>3</v>
-      </c>
-      <c r="F12" s="41" t="s">
-        <v>77</v>
-      </c>
-      <c r="G12" s="1">
+        <v/>
+      </c>
+      <c r="F12" s="41"/>
+      <c r="G12" s="1" t="str">
         <f>_xlfn.IFNA(VLOOKUP(F12,'Base Locations'!$A$1:$F$341,2),"")</f>
-        <v>229786</v>
-      </c>
-      <c r="H12" s="41" t="s">
-        <v>77</v>
-      </c>
+        <v/>
+      </c>
+      <c r="H12" s="41"/>
       <c r="I12" s="1" t="str">
         <f>_xlfn.IFNA(VLOOKUP(H12,'Base Locations'!A11:F351,2),"")</f>
         <v/>
       </c>
-      <c r="J12" s="41" t="s">
-        <v>1198</v>
-      </c>
-      <c r="K12" s="41" t="s">
-        <v>409</v>
-      </c>
+      <c r="J12" s="41"/>
+      <c r="K12" s="41"/>
       <c r="L12" s="41"/>
-      <c r="M12" s="41" t="s">
-        <v>1169</v>
-      </c>
+      <c r="M12" s="41"/>
       <c r="N12" s="1" t="str">
         <f>_xlfn.IFNA(VLOOKUP(M12,Services!$A$1:$B$45,2),"")</f>
-        <v>BHA3</v>
+        <v/>
       </c>
       <c r="O12" s="41"/>
       <c r="P12" s="1" t="str">
@@ -8751,54 +8686,36 @@
       <c r="AD12" s="41"/>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A13" s="41" t="s">
-        <v>1223</v>
-      </c>
-      <c r="B13" s="41" t="s">
-        <v>1224</v>
-      </c>
-      <c r="C13" s="42" t="s">
-        <v>1225</v>
-      </c>
-      <c r="D13" s="41" t="s">
-        <v>5</v>
-      </c>
-      <c r="E13" s="1">
+      <c r="A13" s="41"/>
+      <c r="B13" s="41"/>
+      <c r="C13" s="42"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="1" t="str">
         <f>_xlfn.IFNA(VLOOKUP(D13,Region!$A$2:$B$11,2),"")</f>
-        <v>3</v>
-      </c>
-      <c r="F13" s="41" t="s">
-        <v>78</v>
-      </c>
-      <c r="G13" s="1">
+        <v/>
+      </c>
+      <c r="F13" s="41"/>
+      <c r="G13" s="1" t="str">
         <f>_xlfn.IFNA(VLOOKUP(F13,'Base Locations'!$A$1:$F$341,2),"")</f>
-        <v>574546</v>
+        <v/>
       </c>
       <c r="H13" s="41"/>
       <c r="I13" s="1" t="str">
         <f>_xlfn.IFNA(VLOOKUP(H13,'Base Locations'!A12:F352,2),"")</f>
         <v/>
       </c>
-      <c r="J13" s="41" t="s">
-        <v>1198</v>
-      </c>
-      <c r="K13" s="41" t="s">
-        <v>409</v>
-      </c>
+      <c r="J13" s="41"/>
+      <c r="K13" s="41"/>
       <c r="L13" s="41"/>
-      <c r="M13" s="41" t="s">
-        <v>13</v>
-      </c>
+      <c r="M13" s="41"/>
       <c r="N13" s="1" t="str">
         <f>_xlfn.IFNA(VLOOKUP(M13,Services!$A$1:$B$45,2),"")</f>
-        <v>BAB1</v>
-      </c>
-      <c r="O13" s="41" t="s">
-        <v>13</v>
-      </c>
+        <v/>
+      </c>
+      <c r="O13" s="41"/>
       <c r="P13" s="1" t="str">
         <f>_xlfn.IFNA(VLOOKUP(O13,Services!$A$1:$B$45,2),"")</f>
-        <v>BAB1</v>
+        <v/>
       </c>
       <c r="Q13" s="41"/>
       <c r="R13" s="1" t="str">

</xml_diff>

<commit_message>
refactor: recovered missed cases by previous merges
</commit_message>
<xml_diff>
--- a/src/integrationTest/resources/Staff Data Upload With Jsr.xlsx
+++ b/src/integrationTest/resources/Staff Data Upload With Jsr.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m_224557/Documents/GitHub/duplicate/rd-caseworker-ref-api/src/integrationTest/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/350950/HMCTS/rd-caseworker-ref-api/src/integrationTest/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63F151EA-A49C-C640-B6C0-752013FCD8EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C70A9CC9-57AC-CB44-9ACD-17CB4275DFFF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19540" activeTab="2" xr2:uid="{C3779BBE-D7A5-4756-9223-DEADF9C5B8AB}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14500" activeTab="2" xr2:uid="{C3779BBE-D7A5-4756-9223-DEADF9C5B8AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Guidance" sheetId="11" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1919" uniqueCount="1203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1947" uniqueCount="1215">
   <si>
     <t>Region</t>
   </si>
@@ -3652,7 +3652,43 @@
     <t>test1@justice.gov.uk</t>
   </si>
   <si>
-    <t>test1@domain.com</t>
+    <t>testy</t>
+  </si>
+  <si>
+    <t>tewsyt</t>
+  </si>
+  <si>
+    <t>test2@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>test3@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>test4@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>test5@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>test6@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>test7@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>test8@domain.com</t>
+  </si>
+  <si>
+    <t>test9@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>test10@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>test11@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>test12@justice.gov.uk</t>
   </si>
 </sst>
 </file>
@@ -7651,7 +7687,7 @@
   <dimension ref="A1:AD50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7875,7 +7911,7 @@
         <v>1200</v>
       </c>
       <c r="C3" s="42" t="s">
-        <v>1201</v>
+        <v>1204</v>
       </c>
       <c r="D3" s="41" t="s">
         <v>6</v>
@@ -7954,7 +7990,7 @@
         <v>1200</v>
       </c>
       <c r="C4" s="42" t="s">
-        <v>1201</v>
+        <v>1205</v>
       </c>
       <c r="D4" s="41" t="s">
         <v>10</v>
@@ -8033,7 +8069,7 @@
         <v>1200</v>
       </c>
       <c r="C5" s="42" t="s">
-        <v>1201</v>
+        <v>1206</v>
       </c>
       <c r="D5" s="41" t="s">
         <v>10</v>
@@ -8112,7 +8148,7 @@
         <v>1200</v>
       </c>
       <c r="C6" s="42" t="s">
-        <v>1201</v>
+        <v>1207</v>
       </c>
       <c r="D6" s="41" t="s">
         <v>11</v>
@@ -8191,7 +8227,7 @@
         <v>1200</v>
       </c>
       <c r="C7" s="42" t="s">
-        <v>1201</v>
+        <v>1208</v>
       </c>
       <c r="D7" s="41" t="s">
         <v>10</v>
@@ -8270,7 +8306,7 @@
       </c>
       <c r="B8" s="41"/>
       <c r="C8" s="42" t="s">
-        <v>1201</v>
+        <v>1209</v>
       </c>
       <c r="D8" s="41" t="s">
         <v>9</v>
@@ -8351,7 +8387,7 @@
         <v>1200</v>
       </c>
       <c r="C9" s="42" t="s">
-        <v>1202</v>
+        <v>1210</v>
       </c>
       <c r="D9" s="41" t="s">
         <v>10</v>
@@ -8432,7 +8468,7 @@
         <v>1200</v>
       </c>
       <c r="C10" s="42" t="s">
-        <v>1201</v>
+        <v>1211</v>
       </c>
       <c r="D10" s="41"/>
       <c r="E10" s="1" t="str">
@@ -8504,31 +8540,51 @@
       <c r="AD10" s="41"/>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A11" s="41"/>
-      <c r="B11" s="41"/>
-      <c r="C11" s="42"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="1" t="str">
+      <c r="A11" s="41" t="s">
+        <v>1200</v>
+      </c>
+      <c r="B11" s="41" t="s">
+        <v>1200</v>
+      </c>
+      <c r="C11" s="42" t="s">
+        <v>1212</v>
+      </c>
+      <c r="D11" s="41" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="1">
         <f>IF(ISNA(VLOOKUP(D11,Region!$A$2:$B$11,2)),"",VLOOKUP(D11,Region!$A$2:$B$11,2))</f>
-        <v/>
-      </c>
-      <c r="F11" s="41"/>
-      <c r="G11" s="1" t="str">
+        <v>3</v>
+      </c>
+      <c r="F11" s="41" t="s">
+        <v>70</v>
+      </c>
+      <c r="G11" s="1">
         <f>IF(ISNA(VLOOKUP(F11,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F11,'Base Locations'!$A$1:$F$341,2))</f>
-        <v/>
-      </c>
-      <c r="H11" s="41"/>
+        <v>827534</v>
+      </c>
+      <c r="H11" s="41" t="s">
+        <v>70</v>
+      </c>
       <c r="I11" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(H11,'Base Locations'!A10:F350,2)),"",VLOOKUP(H11,'Base Locations'!A10:F350,2))</f>
         <v/>
       </c>
-      <c r="J11" s="41"/>
-      <c r="K11" s="41"/>
-      <c r="L11" s="41"/>
-      <c r="M11" s="41"/>
+      <c r="J11" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="K11" s="41" t="s">
+        <v>408</v>
+      </c>
+      <c r="L11" s="41" t="s">
+        <v>409</v>
+      </c>
+      <c r="M11" s="41" t="s">
+        <v>1168</v>
+      </c>
       <c r="N11" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(M11,Services!$A$1:$B$45,2)),"",VLOOKUP(M11,Services!$A$1:$B$45,2))</f>
-        <v/>
+        <v>BAB2</v>
       </c>
       <c r="O11" s="41"/>
       <c r="P11" s="1" t="str">
@@ -8569,31 +8625,49 @@
       <c r="AD11" s="41"/>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A12" s="41"/>
-      <c r="B12" s="41"/>
-      <c r="C12" s="42"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="1" t="str">
+      <c r="A12" s="41" t="s">
+        <v>1202</v>
+      </c>
+      <c r="B12" s="41" t="s">
+        <v>1203</v>
+      </c>
+      <c r="C12" s="42" t="s">
+        <v>1213</v>
+      </c>
+      <c r="D12" s="41" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="1">
         <f>IF(ISNA(VLOOKUP(D12,Region!$A$2:$B$11,2)),"",VLOOKUP(D12,Region!$A$2:$B$11,2))</f>
-        <v/>
-      </c>
-      <c r="F12" s="41"/>
-      <c r="G12" s="1" t="str">
+        <v>3</v>
+      </c>
+      <c r="F12" s="41" t="s">
+        <v>72</v>
+      </c>
+      <c r="G12" s="1">
         <f>IF(ISNA(VLOOKUP(F12,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F12,'Base Locations'!$A$1:$F$341,2))</f>
-        <v/>
+        <v>271588</v>
       </c>
       <c r="H12" s="41"/>
       <c r="I12" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(H12,'Base Locations'!A11:F351,2)),"",VLOOKUP(H12,'Base Locations'!A11:F351,2))</f>
         <v/>
       </c>
-      <c r="J12" s="41"/>
-      <c r="K12" s="41"/>
-      <c r="L12" s="41"/>
-      <c r="M12" s="41"/>
+      <c r="J12" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="K12" s="41" t="s">
+        <v>409</v>
+      </c>
+      <c r="L12" s="41" t="s">
+        <v>409</v>
+      </c>
+      <c r="M12" s="41" t="s">
+        <v>13</v>
+      </c>
       <c r="N12" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(M12,Services!$A$1:$B$45,2)),"",VLOOKUP(M12,Services!$A$1:$B$45,2))</f>
-        <v/>
+        <v>BAB1</v>
       </c>
       <c r="O12" s="41"/>
       <c r="P12" s="1" t="str">
@@ -8634,36 +8708,54 @@
       <c r="AD12" s="41"/>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A13" s="41"/>
-      <c r="B13" s="41"/>
-      <c r="C13" s="42"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="1" t="str">
+      <c r="A13" s="41" t="s">
+        <v>1200</v>
+      </c>
+      <c r="B13" s="41" t="s">
+        <v>1200</v>
+      </c>
+      <c r="C13" s="42" t="s">
+        <v>1214</v>
+      </c>
+      <c r="D13" s="41" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="1">
         <f>IF(ISNA(VLOOKUP(D13,Region!$A$2:$B$11,2)),"",VLOOKUP(D13,Region!$A$2:$B$11,2))</f>
-        <v/>
-      </c>
-      <c r="F13" s="41"/>
-      <c r="G13" s="1" t="str">
+        <v>3</v>
+      </c>
+      <c r="F13" s="41" t="s">
+        <v>73</v>
+      </c>
+      <c r="G13" s="1">
         <f>IF(ISNA(VLOOKUP(F13,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F13,'Base Locations'!$A$1:$F$341,2))</f>
-        <v/>
+        <v>239985</v>
       </c>
       <c r="H13" s="41"/>
       <c r="I13" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(H13,'Base Locations'!A12:F352,2)),"",VLOOKUP(H13,'Base Locations'!A12:F352,2))</f>
         <v/>
       </c>
-      <c r="J13" s="41"/>
-      <c r="K13" s="41"/>
+      <c r="J13" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="K13" s="41" t="s">
+        <v>409</v>
+      </c>
       <c r="L13" s="41"/>
-      <c r="M13" s="41"/>
+      <c r="M13" s="41" t="s">
+        <v>13</v>
+      </c>
       <c r="N13" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(M13,Services!$A$1:$B$45,2)),"",VLOOKUP(M13,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O13" s="41"/>
+        <v>BAB1</v>
+      </c>
+      <c r="O13" s="41" t="s">
+        <v>13</v>
+      </c>
       <c r="P13" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(O13,Services!$A$1:$B$45,2)),"",VLOOKUP(O13,Services!$A$1:$B$45,2))</f>
-        <v/>
+        <v>BAB1</v>
       </c>
       <c r="Q13" s="41"/>
       <c r="R13" s="1" t="str">

</xml_diff>

<commit_message>
RDCC-2483: adding validation for primary location field
</commit_message>
<xml_diff>
--- a/src/integrationTest/resources/Staff Data Upload With Jsr.xlsx
+++ b/src/integrationTest/resources/Staff Data Upload With Jsr.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/350950/HMCTS/rd-caseworker-ref-api/src/integrationTest/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m_900458/Documents/HMCTS/rd-caseworker-ref-api/src/integrationTest/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C70A9CC9-57AC-CB44-9ACD-17CB4275DFFF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3027B103-6C81-874F-B95E-13CC792F9D8C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14500" activeTab="2" xr2:uid="{C3779BBE-D7A5-4756-9223-DEADF9C5B8AB}"/>
   </bookViews>
@@ -28,20 +28,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1947" uniqueCount="1215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1955" uniqueCount="1216">
   <si>
     <t>Region</t>
   </si>
@@ -3689,6 +3681,9 @@
   </si>
   <si>
     <t>test12@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>test13@justice.gov.uk</t>
   </si>
 </sst>
 </file>
@@ -7687,7 +7682,7 @@
   <dimension ref="A1:AD50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8791,31 +8786,47 @@
       <c r="AD13" s="41"/>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A14" s="41"/>
-      <c r="B14" s="41"/>
-      <c r="C14" s="42"/>
-      <c r="D14" s="41"/>
-      <c r="E14" s="1" t="str">
+      <c r="A14" s="41" t="s">
+        <v>1200</v>
+      </c>
+      <c r="B14" s="41" t="s">
+        <v>1200</v>
+      </c>
+      <c r="C14" s="42" t="s">
+        <v>1215</v>
+      </c>
+      <c r="D14" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14" s="1">
         <f>IF(ISNA(VLOOKUP(D14,Region!$A$2:$B$11,2)),"",VLOOKUP(D14,Region!$A$2:$B$11,2))</f>
-        <v/>
+        <v>2</v>
       </c>
       <c r="F14" s="41"/>
       <c r="G14" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(F14,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F14,'Base Locations'!$A$1:$F$341,2))</f>
         <v/>
       </c>
-      <c r="H14" s="41"/>
-      <c r="I14" s="1" t="str">
+      <c r="H14" s="41" t="s">
+        <v>86</v>
+      </c>
+      <c r="I14" s="1">
         <f>IF(ISNA(VLOOKUP(H14,'Base Locations'!A13:F353,2)),"",VLOOKUP(H14,'Base Locations'!A13:F353,2))</f>
-        <v/>
-      </c>
-      <c r="J14" s="41"/>
-      <c r="K14" s="41"/>
+        <v>500233</v>
+      </c>
+      <c r="J14" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="K14" s="41" t="s">
+        <v>408</v>
+      </c>
       <c r="L14" s="41"/>
-      <c r="M14" s="41"/>
+      <c r="M14" s="41" t="s">
+        <v>1168</v>
+      </c>
       <c r="N14" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(M14,Services!$A$1:$B$45,2)),"",VLOOKUP(M14,Services!$A$1:$B$45,2))</f>
-        <v/>
+        <v>BAB2</v>
       </c>
       <c r="O14" s="41"/>
       <c r="P14" s="1" t="str">

</xml_diff>

<commit_message>
RDCC-2509: amending test case
</commit_message>
<xml_diff>
--- a/src/integrationTest/resources/Staff Data Upload With Jsr.xlsx
+++ b/src/integrationTest/resources/Staff Data Upload With Jsr.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m_900458/Documents/HMCTS/rd-caseworker-ref-api/src/integrationTest/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/778425/Projects/rd-caseworker-ref-api/src/integrationTest/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3027B103-6C81-874F-B95E-13CC792F9D8C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB7AE003-3ABE-664A-9FCD-F5532AA54C78}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14500" activeTab="2" xr2:uid="{C3779BBE-D7A5-4756-9223-DEADF9C5B8AB}"/>
   </bookViews>
@@ -28,12 +28,21 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1955" uniqueCount="1216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1975" uniqueCount="1219">
   <si>
     <t>Region</t>
   </si>
@@ -3684,6 +3693,15 @@
   </si>
   <si>
     <t>test13@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>asdhjuioiuehasdhjuioiuehasdhjuioiuehasdhjuioiuehasdhjuioiuehasdhjuioiuehasdhjuioiuehasdhjuioiuehasdhjuioiuehasdhjuioiuehlokijuheytydhdjwwd</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>te*st</t>
   </si>
 </sst>
 </file>
@@ -3926,7 +3944,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -4042,6 +4060,9 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -7682,7 +7703,7 @@
   <dimension ref="A1:AD50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8867,36 +8888,56 @@
       <c r="AD14" s="41"/>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A15" s="41"/>
-      <c r="B15" s="41"/>
-      <c r="C15" s="42"/>
-      <c r="D15" s="41"/>
-      <c r="E15" s="1" t="str">
+      <c r="A15" s="41" t="s">
+        <v>1216</v>
+      </c>
+      <c r="B15" s="41" t="s">
+        <v>1200</v>
+      </c>
+      <c r="C15" s="42" t="s">
+        <v>1215</v>
+      </c>
+      <c r="D15" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" s="1">
         <f>IF(ISNA(VLOOKUP(D15,Region!$A$2:$B$11,2)),"",VLOOKUP(D15,Region!$A$2:$B$11,2))</f>
-        <v/>
-      </c>
-      <c r="F15" s="41"/>
-      <c r="G15" s="1" t="str">
+        <v>2</v>
+      </c>
+      <c r="F15" s="44" t="s">
+        <v>73</v>
+      </c>
+      <c r="G15" s="1">
         <f>IF(ISNA(VLOOKUP(F15,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F15,'Base Locations'!$A$1:$F$341,2))</f>
-        <v/>
-      </c>
-      <c r="H15" s="41"/>
-      <c r="I15" s="1" t="str">
+        <v>239985</v>
+      </c>
+      <c r="H15" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="I15" s="1">
         <f>IF(ISNA(VLOOKUP(H15,'Base Locations'!A14:F354,2)),"",VLOOKUP(H15,'Base Locations'!A14:F354,2))</f>
-        <v/>
-      </c>
-      <c r="J15" s="41"/>
-      <c r="K15" s="41"/>
+        <v>500233</v>
+      </c>
+      <c r="J15" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="K15" s="41" t="s">
+        <v>408</v>
+      </c>
       <c r="L15" s="41"/>
-      <c r="M15" s="41"/>
+      <c r="M15" s="44" t="s">
+        <v>1168</v>
+      </c>
       <c r="N15" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(M15,Services!$A$1:$B$45,2)),"",VLOOKUP(M15,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O15" s="41"/>
+        <v>BAB2</v>
+      </c>
+      <c r="O15" s="41" t="s">
+        <v>13</v>
+      </c>
       <c r="P15" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(O15,Services!$A$1:$B$45,2)),"",VLOOKUP(O15,Services!$A$1:$B$45,2))</f>
-        <v/>
+        <v>BAB1</v>
       </c>
       <c r="Q15" s="41"/>
       <c r="R15" s="1" t="str">
@@ -8932,36 +8973,56 @@
       <c r="AD15" s="41"/>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A16" s="41"/>
-      <c r="B16" s="41"/>
-      <c r="C16" s="42"/>
-      <c r="D16" s="41"/>
-      <c r="E16" s="1" t="str">
+      <c r="A16" s="41" t="s">
+        <v>1217</v>
+      </c>
+      <c r="B16" s="41" t="s">
+        <v>1218</v>
+      </c>
+      <c r="C16" s="42" t="s">
+        <v>1215</v>
+      </c>
+      <c r="D16" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" s="1">
         <f>IF(ISNA(VLOOKUP(D16,Region!$A$2:$B$11,2)),"",VLOOKUP(D16,Region!$A$2:$B$11,2))</f>
-        <v/>
-      </c>
-      <c r="F16" s="41"/>
-      <c r="G16" s="1" t="str">
+        <v>2</v>
+      </c>
+      <c r="F16" s="44" t="s">
+        <v>73</v>
+      </c>
+      <c r="G16" s="1">
         <f>IF(ISNA(VLOOKUP(F16,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F16,'Base Locations'!$A$1:$F$341,2))</f>
-        <v/>
-      </c>
-      <c r="H16" s="41"/>
-      <c r="I16" s="1" t="str">
+        <v>239985</v>
+      </c>
+      <c r="H16" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="I16" s="1">
         <f>IF(ISNA(VLOOKUP(H16,'Base Locations'!A15:F355,2)),"",VLOOKUP(H16,'Base Locations'!A15:F355,2))</f>
-        <v/>
-      </c>
-      <c r="J16" s="41"/>
-      <c r="K16" s="41"/>
+        <v>500233</v>
+      </c>
+      <c r="J16" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="K16" s="41" t="s">
+        <v>408</v>
+      </c>
       <c r="L16" s="41"/>
-      <c r="M16" s="41"/>
+      <c r="M16" s="44" t="s">
+        <v>1168</v>
+      </c>
       <c r="N16" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(M16,Services!$A$1:$B$45,2)),"",VLOOKUP(M16,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O16" s="41"/>
+        <v>BAB2</v>
+      </c>
+      <c r="O16" s="44" t="s">
+        <v>13</v>
+      </c>
       <c r="P16" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(O16,Services!$A$1:$B$45,2)),"",VLOOKUP(O16,Services!$A$1:$B$45,2))</f>
-        <v/>
+        <v>BAB1</v>
       </c>
       <c r="Q16" s="41"/>
       <c r="R16" s="1" t="str">
@@ -11223,7 +11284,7 @@
           <x14:formula1>
             <xm:f>Services!$A$1:$A$43</xm:f>
           </x14:formula1>
-          <xm:sqref>Q2:Q50 S2:S50 U2:U50 W2:W50 Y2:Y50 AA2:AA50 M2:M50 O2:O50</xm:sqref>
+          <xm:sqref>Q2:Q50 S2:S50 U2:U50 W2:W50 Y2:Y50 AA2:AA50 M2:M14 M17:M50 O2:O15 O17:O50</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{69AD3E96-9986-4437-A6D2-54EE41465A4B}">
           <x14:formula1>
@@ -11235,7 +11296,7 @@
           <x14:formula1>
             <xm:f>'Base Locations'!$A$2:$A$341</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:H50 F2:F50</xm:sqref>
+          <xm:sqref>F16:F50 F2:F14 H2:H14 H16:H50</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9447D6FF-71AD-498D-86D2-ECD016FD5810}">
           <x14:formula1>

</xml_diff>

<commit_message>
RDCC-2510: updating tests file with invalid records
</commit_message>
<xml_diff>
--- a/src/integrationTest/resources/Staff Data Upload With Jsr.xlsx
+++ b/src/integrationTest/resources/Staff Data Upload With Jsr.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m_900458/Documents/HMCTS/rd-caseworker-ref-api/src/integrationTest/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m_900458/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE912724-9016-9840-BDC3-7DA468098839}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CF976E54-D203-1F4C-8AD1-190D815BCA3D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14500" activeTab="2" xr2:uid="{C3779BBE-D7A5-4756-9223-DEADF9C5B8AB}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1964" uniqueCount="1217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1985" uniqueCount="1220">
   <si>
     <t>Region</t>
   </si>
@@ -3684,6 +3684,15 @@
   </si>
   <si>
     <t>test13@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>asdhjuioiuehasdhjuioiuehasdhjuioiuehasdhjuioiuehasdhjuioiuehasdhjuioiuehasdhjuioiuehasdhjuioiuehasdhjuioiuehasdhjuioiuehlokijuheytydhdjwwd</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>te*st</t>
   </si>
   <si>
     <t>£$%qw@justice.gov.uk</t>
@@ -3929,7 +3938,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -4045,6 +4054,9 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -7685,7 +7697,7 @@
   <dimension ref="A1:AD50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="O16" sqref="O16:O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8871,34 +8883,34 @@
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A15" s="41" t="s">
-        <v>1200</v>
+        <v>1216</v>
       </c>
       <c r="B15" s="41" t="s">
         <v>1200</v>
       </c>
       <c r="C15" s="42" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="D15" s="41" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E15" s="1">
         <f>IF(ISNA(VLOOKUP(D15,Region!$A$2:$B$11,2)),"",VLOOKUP(D15,Region!$A$2:$B$11,2))</f>
-        <v>5</v>
-      </c>
-      <c r="F15" s="41" t="s">
+        <v>2</v>
+      </c>
+      <c r="F15" s="44" t="s">
         <v>73</v>
       </c>
       <c r="G15" s="1">
         <f>IF(ISNA(VLOOKUP(F15,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F15,'Base Locations'!$A$1:$F$341,2))</f>
         <v>239985</v>
       </c>
-      <c r="H15" s="41" t="s">
-        <v>74</v>
-      </c>
-      <c r="I15" s="1" t="str">
+      <c r="H15" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="I15" s="1">
         <f>IF(ISNA(VLOOKUP(H15,'Base Locations'!A14:F354,2)),"",VLOOKUP(H15,'Base Locations'!A14:F354,2))</f>
-        <v/>
+        <v>500233</v>
       </c>
       <c r="J15" s="41" t="s">
         <v>52</v>
@@ -8907,17 +8919,19 @@
         <v>408</v>
       </c>
       <c r="L15" s="41"/>
-      <c r="M15" s="41" t="s">
-        <v>1169</v>
+      <c r="M15" s="44" t="s">
+        <v>1168</v>
       </c>
       <c r="N15" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(M15,Services!$A$1:$B$45,2)),"",VLOOKUP(M15,Services!$A$1:$B$45,2))</f>
-        <v>BHA3</v>
-      </c>
-      <c r="O15" s="41"/>
+        <v>BAB2</v>
+      </c>
+      <c r="O15" s="41" t="s">
+        <v>13</v>
+      </c>
       <c r="P15" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(O15,Services!$A$1:$B$45,2)),"",VLOOKUP(O15,Services!$A$1:$B$45,2))</f>
-        <v/>
+        <v>BAB1</v>
       </c>
       <c r="Q15" s="41"/>
       <c r="R15" s="1" t="str">
@@ -8953,36 +8967,56 @@
       <c r="AD15" s="41"/>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A16" s="41"/>
-      <c r="B16" s="41"/>
-      <c r="C16" s="42"/>
-      <c r="D16" s="41"/>
-      <c r="E16" s="1" t="str">
+      <c r="A16" s="41" t="s">
+        <v>1217</v>
+      </c>
+      <c r="B16" s="41" t="s">
+        <v>1218</v>
+      </c>
+      <c r="C16" s="42" t="s">
+        <v>1215</v>
+      </c>
+      <c r="D16" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" s="1">
         <f>IF(ISNA(VLOOKUP(D16,Region!$A$2:$B$11,2)),"",VLOOKUP(D16,Region!$A$2:$B$11,2))</f>
-        <v/>
-      </c>
-      <c r="F16" s="41"/>
-      <c r="G16" s="1" t="str">
+        <v>2</v>
+      </c>
+      <c r="F16" s="44" t="s">
+        <v>73</v>
+      </c>
+      <c r="G16" s="1">
         <f>IF(ISNA(VLOOKUP(F16,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F16,'Base Locations'!$A$1:$F$341,2))</f>
-        <v/>
-      </c>
-      <c r="H16" s="41"/>
-      <c r="I16" s="1" t="str">
+        <v>239985</v>
+      </c>
+      <c r="H16" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="I16" s="1">
         <f>IF(ISNA(VLOOKUP(H16,'Base Locations'!A15:F355,2)),"",VLOOKUP(H16,'Base Locations'!A15:F355,2))</f>
-        <v/>
-      </c>
-      <c r="J16" s="41"/>
-      <c r="K16" s="41"/>
+        <v>500233</v>
+      </c>
+      <c r="J16" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="K16" s="41" t="s">
+        <v>408</v>
+      </c>
       <c r="L16" s="41"/>
-      <c r="M16" s="41"/>
+      <c r="M16" s="44" t="s">
+        <v>1168</v>
+      </c>
       <c r="N16" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(M16,Services!$A$1:$B$45,2)),"",VLOOKUP(M16,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O16" s="41"/>
+        <v>BAB2</v>
+      </c>
+      <c r="O16" s="44" t="s">
+        <v>13</v>
+      </c>
       <c r="P16" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(O16,Services!$A$1:$B$45,2)),"",VLOOKUP(O16,Services!$A$1:$B$45,2))</f>
-        <v/>
+        <v>BAB1</v>
       </c>
       <c r="Q16" s="41"/>
       <c r="R16" s="1" t="str">
@@ -9018,36 +9052,56 @@
       <c r="AD16" s="41"/>
     </row>
     <row r="17" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A17" s="41"/>
-      <c r="B17" s="41"/>
-      <c r="C17" s="42"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="1" t="str">
+      <c r="A17" s="41" t="s">
+        <v>1200</v>
+      </c>
+      <c r="B17" s="41" t="s">
+        <v>1200</v>
+      </c>
+      <c r="C17" s="41" t="s">
+        <v>1219</v>
+      </c>
+      <c r="D17" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="1">
         <f>IF(ISNA(VLOOKUP(D17,Region!$A$2:$B$11,2)),"",VLOOKUP(D17,Region!$A$2:$B$11,2))</f>
-        <v/>
-      </c>
-      <c r="F17" s="41"/>
-      <c r="G17" s="1" t="str">
+        <v>5</v>
+      </c>
+      <c r="F17" s="44" t="s">
+        <v>73</v>
+      </c>
+      <c r="G17" s="1">
         <f>IF(ISNA(VLOOKUP(F17,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F17,'Base Locations'!$A$1:$F$341,2))</f>
-        <v/>
-      </c>
-      <c r="H17" s="41"/>
-      <c r="I17" s="1" t="str">
+        <v>239985</v>
+      </c>
+      <c r="H17" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="I17" s="1">
         <f>IF(ISNA(VLOOKUP(H17,'Base Locations'!A16:F356,2)),"",VLOOKUP(H17,'Base Locations'!A16:F356,2))</f>
-        <v/>
-      </c>
-      <c r="J17" s="41"/>
-      <c r="K17" s="41"/>
+        <v>500233</v>
+      </c>
+      <c r="J17" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="K17" s="41" t="s">
+        <v>408</v>
+      </c>
       <c r="L17" s="41"/>
-      <c r="M17" s="41"/>
+      <c r="M17" s="44" t="s">
+        <v>1168</v>
+      </c>
       <c r="N17" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(M17,Services!$A$1:$B$45,2)),"",VLOOKUP(M17,Services!$A$1:$B$45,2))</f>
-        <v/>
-      </c>
-      <c r="O17" s="41"/>
+        <v>BAB2</v>
+      </c>
+      <c r="O17" s="44" t="s">
+        <v>13</v>
+      </c>
       <c r="P17" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(O17,Services!$A$1:$B$45,2)),"",VLOOKUP(O17,Services!$A$1:$B$45,2))</f>
-        <v/>
+        <v>BAB1</v>
       </c>
       <c r="Q17" s="41"/>
       <c r="R17" s="1" t="str">
@@ -11244,7 +11298,7 @@
           <x14:formula1>
             <xm:f>Services!$A$1:$A$43</xm:f>
           </x14:formula1>
-          <xm:sqref>Q2:Q50 S2:S50 U2:U50 W2:W50 Y2:Y50 AA2:AA50 M2:M50 O2:O50</xm:sqref>
+          <xm:sqref>Q2:Q50 S2:S50 U2:U50 W2:W50 Y2:Y50 AA2:AA50 M2:M14 M17:M50 O2:O15 O17:O50</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{69AD3E96-9986-4437-A6D2-54EE41465A4B}">
           <x14:formula1>
@@ -11256,7 +11310,7 @@
           <x14:formula1>
             <xm:f>'Base Locations'!$A$2:$A$341</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:H50 F2:F50</xm:sqref>
+          <xm:sqref>F16:F50 F2:F14 H2:H14 H16:H50</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9447D6FF-71AD-498D-86D2-ECD016FD5810}">
           <x14:formula1>

</xml_diff>

<commit_message>
RDCC-2509: updating excel file to fix integration test
</commit_message>
<xml_diff>
--- a/src/integrationTest/resources/Staff Data Upload With Jsr.xlsx
+++ b/src/integrationTest/resources/Staff Data Upload With Jsr.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m_900458/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/778425/Projects/rd-caseworker-ref-api/src/integrationTest/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CF976E54-D203-1F4C-8AD1-190D815BCA3D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9C6DAC3-5A8B-6A41-A3F4-1EA338472A8C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14500" activeTab="2" xr2:uid="{C3779BBE-D7A5-4756-9223-DEADF9C5B8AB}"/>
   </bookViews>
@@ -28,12 +28,21 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1985" uniqueCount="1220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1985" uniqueCount="1222">
   <si>
     <t>Region</t>
   </si>
@@ -3686,16 +3695,22 @@
     <t>test13@justice.gov.uk</t>
   </si>
   <si>
-    <t>asdhjuioiuehasdhjuioiuehasdhjuioiuehasdhjuioiuehasdhjuioiuehasdhjuioiuehasdhjuioiuehasdhjuioiuehasdhjuioiuehasdhjuioiuehlokijuheytydhdjwwd</t>
-  </si>
-  <si>
     <t>Test</t>
   </si>
   <si>
-    <t>te*st</t>
-  </si>
-  <si>
     <t>£$%qw@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>test15@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>test14@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>te*&amp;£@$st</t>
+  </si>
+  <si>
+    <t>asdhjuioiuehasdhjuioiuehasdhjuioiuehasdhjuioiuehasdhjuioiuehasdhjuioiuehasdhjuioiuehasdhjuioiuehasdhjuioiuehasdhjuioiuehlokijuheytydhdjwwdhhhhh</t>
   </si>
 </sst>
 </file>
@@ -7697,7 +7712,7 @@
   <dimension ref="A1:AD50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16:O17"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8883,13 +8898,13 @@
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A15" s="41" t="s">
-        <v>1216</v>
+        <v>1221</v>
       </c>
       <c r="B15" s="41" t="s">
         <v>1200</v>
       </c>
       <c r="C15" s="42" t="s">
-        <v>1215</v>
+        <v>1219</v>
       </c>
       <c r="D15" s="41" t="s">
         <v>4</v>
@@ -8968,13 +8983,13 @@
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A16" s="41" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="B16" s="41" t="s">
+        <v>1220</v>
+      </c>
+      <c r="C16" s="42" t="s">
         <v>1218</v>
-      </c>
-      <c r="C16" s="42" t="s">
-        <v>1215</v>
       </c>
       <c r="D16" s="41" t="s">
         <v>4</v>
@@ -9059,7 +9074,7 @@
         <v>1200</v>
       </c>
       <c r="C17" s="41" t="s">
-        <v>1219</v>
+        <v>1217</v>
       </c>
       <c r="D17" s="41" t="s">
         <v>9</v>

</xml_diff>